<commit_message>
issue fixed and added validation
</commit_message>
<xml_diff>
--- a/Presentation/Visitor.API/FormatFiles/Template_User.xlsx
+++ b/Presentation/Visitor.API/FormatFiles/Template_User.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sujay\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D67AE9D-474D-477A-B9EB-4286C7F61105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AP$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AQ$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
   <si>
     <t>UserCode</t>
   </si>
@@ -305,12 +299,18 @@
   </si>
   <si>
     <t>SuperAdmin</t>
+  </si>
+  <si>
+    <t>CHOWGULE LAVGAN</t>
+  </si>
+  <si>
+    <t>Branch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -734,53 +734,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="13.88671875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="13.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="16" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" style="2" customWidth="1"/>
-    <col min="14" max="16" width="16.5546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.33203125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="25.33203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10.6640625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8" style="3" customWidth="1"/>
-    <col min="28" max="28" width="19.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="16.5546875" style="3" customWidth="1"/>
-    <col min="40" max="40" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="3" customWidth="1"/>
+    <col min="11" max="12" width="16.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="2" customWidth="1"/>
+    <col min="15" max="17" width="16.5703125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.28515625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.7109375" style="3" customWidth="1"/>
+    <col min="26" max="26" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" style="3" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="16.5703125" style="3" customWidth="1"/>
+    <col min="41" max="41" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:43">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -815,100 +815,103 @@
         <v>8</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AK1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AM1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -942,83 +945,83 @@
       <c r="K2" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>72</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="Q2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="R2" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="T2" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="U2" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="U2" s="19">
+      <c r="V2" s="19">
         <v>5</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="W2" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AD2" s="16" t="s">
+      <c r="AE2" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AJ2" s="17" t="s">
+      <c r="AK2" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="AK2" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="AL2" s="8" t="s">
         <v>57</v>
@@ -1026,17 +1029,20 @@
       <c r="AM2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AN2" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AN2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO2" s="18" t="s">
         <v>82</v>
       </c>
       <c r="AP2" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:42">
+      <c r="AQ2" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1070,83 +1076,83 @@
       <c r="K3" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>72</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="Q3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="R3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="T3" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="U3" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="U3" s="19">
+      <c r="V3" s="19">
         <v>10</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="W3" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AD3" s="16" t="s">
+      <c r="AE3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AJ3" s="17" t="s">
+      <c r="AK3" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="AK3" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="AL3" s="8" t="s">
         <v>57</v>
@@ -1155,7 +1161,7 @@
         <v>57</v>
       </c>
       <c r="AN3" s="8" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="AO3" s="8" t="s">
         <v>82</v>
@@ -1163,364 +1169,374 @@
       <c r="AP3" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:42">
+      <c r="AQ3" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43">
       <c r="J4" s="1"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="9"/>
+      <c r="L4" s="2"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="2"/>
+      <c r="N4" s="9"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="21"/>
-      <c r="S4" s="1"/>
-      <c r="Y4" s="3"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="21"/>
+      <c r="T4" s="1"/>
       <c r="Z4" s="3"/>
-      <c r="AE4" s="3"/>
+      <c r="AA4" s="3"/>
       <c r="AF4" s="3"/>
-      <c r="AH4" s="3"/>
+      <c r="AG4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
-      <c r="AK4" s="2"/>
+      <c r="AK4" s="3"/>
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
-    </row>
-    <row r="5" spans="1:42">
+      <c r="AN4" s="2"/>
+    </row>
+    <row r="5" spans="1:43">
       <c r="J5" s="1"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="9"/>
+      <c r="L5" s="2"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="9"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="21"/>
-      <c r="S5" s="1"/>
-      <c r="Y5" s="3"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="21"/>
+      <c r="T5" s="1"/>
       <c r="Z5" s="3"/>
-      <c r="AE5" s="3"/>
+      <c r="AA5" s="3"/>
       <c r="AF5" s="3"/>
-      <c r="AH5" s="3"/>
+      <c r="AG5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
-      <c r="AK5" s="2"/>
+      <c r="AK5" s="3"/>
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
-    </row>
-    <row r="6" spans="1:42">
+      <c r="AN5" s="2"/>
+    </row>
+    <row r="6" spans="1:43">
       <c r="J6" s="1"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="9"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="2"/>
+      <c r="N6" s="9"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="21"/>
-      <c r="S6" s="1"/>
-      <c r="Y6" s="3"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="21"/>
+      <c r="T6" s="1"/>
       <c r="Z6" s="3"/>
-      <c r="AE6" s="3"/>
+      <c r="AA6" s="3"/>
       <c r="AF6" s="3"/>
-      <c r="AH6" s="3"/>
+      <c r="AG6" s="3"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
-      <c r="AK6" s="2"/>
+      <c r="AK6" s="3"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
-    </row>
-    <row r="7" spans="1:42">
+      <c r="AN6" s="2"/>
+    </row>
+    <row r="7" spans="1:43">
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="9"/>
+      <c r="L7" s="2"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="2"/>
+      <c r="N7" s="9"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="21"/>
-      <c r="S7" s="1"/>
-      <c r="Y7" s="3"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="21"/>
+      <c r="T7" s="1"/>
       <c r="Z7" s="3"/>
-      <c r="AE7" s="3"/>
+      <c r="AA7" s="3"/>
       <c r="AF7" s="3"/>
-      <c r="AH7" s="3"/>
+      <c r="AG7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
-      <c r="AK7" s="2"/>
+      <c r="AK7" s="3"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
-    </row>
-    <row r="8" spans="1:42">
+      <c r="AN7" s="2"/>
+    </row>
+    <row r="8" spans="1:43">
       <c r="J8" s="1"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="9"/>
+      <c r="L8" s="2"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="9"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-      <c r="Q8" s="21"/>
-      <c r="S8" s="1"/>
-      <c r="Y8" s="3"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="21"/>
+      <c r="T8" s="1"/>
       <c r="Z8" s="3"/>
-      <c r="AE8" s="3"/>
+      <c r="AA8" s="3"/>
       <c r="AF8" s="3"/>
-      <c r="AH8" s="3"/>
+      <c r="AG8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
-      <c r="AK8" s="2"/>
+      <c r="AK8" s="3"/>
       <c r="AL8" s="2"/>
       <c r="AM8" s="2"/>
-    </row>
-    <row r="9" spans="1:42">
+      <c r="AN8" s="2"/>
+    </row>
+    <row r="9" spans="1:43">
       <c r="J9" s="1"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="9"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="2"/>
+      <c r="N9" s="9"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="21"/>
-      <c r="S9" s="1"/>
-      <c r="Y9" s="3"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="21"/>
+      <c r="T9" s="1"/>
       <c r="Z9" s="3"/>
-      <c r="AE9" s="3"/>
+      <c r="AA9" s="3"/>
       <c r="AF9" s="3"/>
-      <c r="AH9" s="3"/>
+      <c r="AG9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
-      <c r="AK9" s="2"/>
+      <c r="AK9" s="3"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
-    </row>
-    <row r="10" spans="1:42">
+      <c r="AN9" s="2"/>
+    </row>
+    <row r="10" spans="1:43">
       <c r="J10" s="1"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="9"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="2"/>
+      <c r="N10" s="9"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="21"/>
-      <c r="S10" s="1"/>
-      <c r="Y10" s="3"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="21"/>
+      <c r="T10" s="1"/>
       <c r="Z10" s="3"/>
-      <c r="AE10" s="3"/>
+      <c r="AA10" s="3"/>
       <c r="AF10" s="3"/>
-      <c r="AH10" s="3"/>
+      <c r="AG10" s="3"/>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="3"/>
-      <c r="AK10" s="2"/>
+      <c r="AK10" s="3"/>
       <c r="AL10" s="2"/>
       <c r="AM10" s="2"/>
-    </row>
-    <row r="11" spans="1:42">
-      <c r="L11" s="10"/>
+      <c r="AN10" s="2"/>
+    </row>
+    <row r="11" spans="1:43">
       <c r="M11" s="10"/>
-      <c r="Q11" s="21"/>
-    </row>
-    <row r="12" spans="1:42">
-      <c r="L12" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="R11" s="21"/>
+    </row>
+    <row r="12" spans="1:43">
       <c r="M12" s="10"/>
-      <c r="Q12" s="21"/>
-    </row>
-    <row r="13" spans="1:42">
-      <c r="L13" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="R12" s="21"/>
+    </row>
+    <row r="13" spans="1:43">
       <c r="M13" s="10"/>
-      <c r="Q13" s="21"/>
-    </row>
-    <row r="14" spans="1:42">
-      <c r="L14" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="R13" s="21"/>
+    </row>
+    <row r="14" spans="1:43">
       <c r="M14" s="10"/>
-      <c r="Q14" s="21"/>
-    </row>
-    <row r="15" spans="1:42">
-      <c r="L15" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="R14" s="21"/>
+    </row>
+    <row r="15" spans="1:43">
       <c r="M15" s="10"/>
-      <c r="Q15" s="21"/>
-    </row>
-    <row r="16" spans="1:42">
-      <c r="L16" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="R15" s="21"/>
+    </row>
+    <row r="16" spans="1:43">
       <c r="M16" s="10"/>
-      <c r="Q16" s="21"/>
-    </row>
-    <row r="17" spans="12:17">
-      <c r="L17" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="R16" s="21"/>
+    </row>
+    <row r="17" spans="13:18">
       <c r="M17" s="10"/>
-      <c r="Q17" s="21"/>
-    </row>
-    <row r="18" spans="12:17">
-      <c r="L18" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="R17" s="21"/>
+    </row>
+    <row r="18" spans="13:18">
       <c r="M18" s="10"/>
-      <c r="Q18" s="21"/>
-    </row>
-    <row r="19" spans="12:17">
-      <c r="L19" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="R18" s="21"/>
+    </row>
+    <row r="19" spans="13:18">
       <c r="M19" s="10"/>
-      <c r="Q19" s="21"/>
-    </row>
-    <row r="20" spans="12:17">
-      <c r="L20" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="R19" s="21"/>
+    </row>
+    <row r="20" spans="13:18">
       <c r="M20" s="10"/>
-      <c r="Q20" s="21"/>
-    </row>
-    <row r="21" spans="12:17">
-      <c r="L21" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="R20" s="21"/>
+    </row>
+    <row r="21" spans="13:18">
       <c r="M21" s="10"/>
-      <c r="Q21" s="21"/>
-    </row>
-    <row r="22" spans="12:17">
-      <c r="L22" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="R21" s="21"/>
+    </row>
+    <row r="22" spans="13:18">
       <c r="M22" s="10"/>
-      <c r="Q22" s="21"/>
-    </row>
-    <row r="23" spans="12:17">
-      <c r="L23" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="R22" s="21"/>
+    </row>
+    <row r="23" spans="13:18">
       <c r="M23" s="10"/>
-      <c r="Q23" s="21"/>
-    </row>
-    <row r="24" spans="12:17">
-      <c r="L24" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="R23" s="21"/>
+    </row>
+    <row r="24" spans="13:18">
       <c r="M24" s="10"/>
-      <c r="Q24" s="21"/>
-    </row>
-    <row r="25" spans="12:17">
-      <c r="L25" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="R24" s="21"/>
+    </row>
+    <row r="25" spans="13:18">
       <c r="M25" s="10"/>
-      <c r="Q25" s="21"/>
-    </row>
-    <row r="26" spans="12:17">
-      <c r="L26" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="R25" s="21"/>
+    </row>
+    <row r="26" spans="13:18">
       <c r="M26" s="10"/>
-      <c r="Q26" s="21"/>
-    </row>
-    <row r="27" spans="12:17">
-      <c r="L27" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="R26" s="21"/>
+    </row>
+    <row r="27" spans="13:18">
       <c r="M27" s="10"/>
-      <c r="Q27" s="21"/>
-    </row>
-    <row r="28" spans="12:17">
-      <c r="L28" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="R27" s="21"/>
+    </row>
+    <row r="28" spans="13:18">
       <c r="M28" s="10"/>
-      <c r="Q28" s="21"/>
-    </row>
-    <row r="29" spans="12:17">
-      <c r="L29" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="R28" s="21"/>
+    </row>
+    <row r="29" spans="13:18">
       <c r="M29" s="10"/>
-      <c r="Q29" s="21"/>
-    </row>
-    <row r="30" spans="12:17">
-      <c r="L30" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="R29" s="21"/>
+    </row>
+    <row r="30" spans="13:18">
       <c r="M30" s="10"/>
-      <c r="Q30" s="21"/>
-    </row>
-    <row r="31" spans="12:17">
-      <c r="L31" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="R30" s="21"/>
+    </row>
+    <row r="31" spans="13:18">
       <c r="M31" s="10"/>
-      <c r="Q31" s="21"/>
-    </row>
-    <row r="32" spans="12:17">
-      <c r="L32" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="R31" s="21"/>
+    </row>
+    <row r="32" spans="13:18">
       <c r="M32" s="10"/>
-      <c r="Q32" s="21"/>
-    </row>
-    <row r="33" spans="12:17">
-      <c r="L33" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="R32" s="21"/>
+    </row>
+    <row r="33" spans="13:18">
       <c r="M33" s="10"/>
-      <c r="Q33" s="21"/>
-    </row>
-    <row r="34" spans="12:17">
-      <c r="L34" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="R33" s="21"/>
+    </row>
+    <row r="34" spans="13:18">
       <c r="M34" s="10"/>
-      <c r="Q34" s="21"/>
-    </row>
-    <row r="35" spans="12:17">
-      <c r="L35" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="R34" s="21"/>
+    </row>
+    <row r="35" spans="13:18">
       <c r="M35" s="10"/>
-      <c r="Q35" s="21"/>
-    </row>
-    <row r="36" spans="12:17">
-      <c r="L36" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="R35" s="21"/>
+    </row>
+    <row r="36" spans="13:18">
       <c r="M36" s="10"/>
-      <c r="Q36" s="21"/>
-    </row>
-    <row r="37" spans="12:17">
-      <c r="L37" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="R36" s="21"/>
+    </row>
+    <row r="37" spans="13:18">
       <c r="M37" s="10"/>
-      <c r="Q37" s="21"/>
-    </row>
-    <row r="38" spans="12:17">
-      <c r="L38" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="R37" s="21"/>
+    </row>
+    <row r="38" spans="13:18">
       <c r="M38" s="10"/>
-      <c r="Q38" s="21"/>
-    </row>
-    <row r="39" spans="12:17">
-      <c r="L39" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="R38" s="21"/>
+    </row>
+    <row r="39" spans="13:18">
       <c r="M39" s="10"/>
-      <c r="Q39" s="21"/>
-    </row>
-    <row r="40" spans="12:17">
-      <c r="L40" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="R39" s="21"/>
+    </row>
+    <row r="40" spans="13:18">
       <c r="M40" s="10"/>
-      <c r="Q40" s="21"/>
-    </row>
-    <row r="41" spans="12:17">
-      <c r="L41" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="R40" s="21"/>
+    </row>
+    <row r="41" spans="13:18">
       <c r="M41" s="10"/>
-      <c r="Q41" s="21"/>
-    </row>
-    <row r="42" spans="12:17">
-      <c r="L42" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="R41" s="21"/>
+    </row>
+    <row r="42" spans="13:18">
       <c r="M42" s="10"/>
-      <c r="Q42" s="21"/>
-    </row>
-    <row r="43" spans="12:17">
-      <c r="L43" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="R42" s="21"/>
+    </row>
+    <row r="43" spans="13:18">
       <c r="M43" s="10"/>
-      <c r="Q43" s="21"/>
-    </row>
-    <row r="44" spans="12:17">
-      <c r="L44" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="R43" s="21"/>
+    </row>
+    <row r="44" spans="13:18">
       <c r="M44" s="10"/>
-      <c r="Q44" s="21"/>
-    </row>
-    <row r="45" spans="12:17">
-      <c r="L45" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="R44" s="21"/>
+    </row>
+    <row r="45" spans="13:18">
       <c r="M45" s="10"/>
-      <c r="Q45" s="21"/>
-    </row>
-    <row r="46" spans="12:17">
-      <c r="L46" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="R45" s="21"/>
+    </row>
+    <row r="46" spans="13:18">
       <c r="M46" s="10"/>
-      <c r="Q46" s="21"/>
-    </row>
-    <row r="47" spans="12:17">
-      <c r="L47" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="R46" s="21"/>
+    </row>
+    <row r="47" spans="13:18">
       <c r="M47" s="10"/>
-      <c r="Q47" s="21"/>
-    </row>
-    <row r="48" spans="12:17">
-      <c r="L48" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="R47" s="21"/>
+    </row>
+    <row r="48" spans="13:18">
       <c r="M48" s="10"/>
-      <c r="Q48" s="21"/>
-    </row>
-    <row r="49" spans="12:17">
-      <c r="L49" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="R48" s="21"/>
+    </row>
+    <row r="49" spans="13:18">
       <c r="M49" s="10"/>
-      <c r="Q49" s="21"/>
+      <c r="N49" s="10"/>
+      <c r="R49" s="21"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL1048576 AB1:AB1048576 AK1:AK1048576 AM1:AM1048576 AP1 AN2:AP1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM1048576 AC1:AC1048576 AL1:AL1048576 AN1:AN1048576 AQ1 AO2:AQ1048576">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{3A47EF66-CCBB-490D-BFB4-E29A5EB9C2BD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
       <formula1>"Male,Female,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3" xr:uid="{EDD800B9-F012-4B87-9768-D558B41E79A0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q3">
       <formula1>"Married,UnMarried,Single"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" tooltip="mailto:email1@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" tooltip="mailto:email2@gmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" tooltip="mailto:email1@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId2" tooltip="mailto:email2@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
issue fixed and email added
</commit_message>
<xml_diff>
--- a/Presentation/Visitor.API/FormatFiles/Template_User.xlsx
+++ b/Presentation/Visitor.API/FormatFiles/Template_User.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AQ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AP$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="93">
   <si>
     <t>UserCode</t>
   </si>
@@ -31,9 +31,6 @@
     <t>EmailId</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -221,12 +218,6 @@
   </si>
   <si>
     <t>IsManager</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin258</t>
   </si>
   <si>
     <t>1</t>
@@ -735,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ49"/>
+  <dimension ref="A1:AP49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -746,41 +737,40 @@
     <col min="2" max="3" width="13.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="3" customWidth="1"/>
-    <col min="11" max="12" width="16.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="2" customWidth="1"/>
-    <col min="15" max="17" width="16.5703125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.28515625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="25.28515625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.7109375" style="3" customWidth="1"/>
-    <col min="26" max="26" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" style="3" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="16.5703125" style="3" customWidth="1"/>
-    <col min="41" max="41" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8" customWidth="1"/>
+    <col min="6" max="6" width="16" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="3" customWidth="1"/>
+    <col min="10" max="11" width="16.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="2" customWidth="1"/>
+    <col min="14" max="16" width="16.5703125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.28515625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="25.28515625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10.7109375" style="3" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8" style="3" customWidth="1"/>
+    <col min="28" max="28" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="16.5703125" style="3" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:42">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -788,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -797,10 +787,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>5</v>
@@ -812,34 +802,34 @@
         <v>7</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="T1" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>58</v>
@@ -848,25 +838,25 @@
         <v>59</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="X1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="AC1" s="6" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="AD1" s="6" t="s">
         <v>62</v>
@@ -881,656 +871,647 @@
         <v>65</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="AI1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="AJ1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN1" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="AK1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM1" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN1" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="AO1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AP1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+    </row>
+    <row r="2" spans="1:42">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:43">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>87</v>
+      <c r="J2" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="U2" s="19">
+        <v>5</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="V2" s="19">
-        <v>5</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y2" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE2" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="AI2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AJ2" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP2" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42">
+      <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="AK2" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AM2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AN2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO2" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP2" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ2" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>88</v>
+      <c r="J3" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="R3" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" s="19">
+        <v>10</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH3" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="U3" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="V3" s="19">
-        <v>10</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE3" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="AI3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AJ3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK3" s="17" t="s">
-        <v>83</v>
+      <c r="AJ3" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK3" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="AL3" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM3" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AN3" s="8" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="AO3" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ3" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43">
-      <c r="J4" s="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42">
+      <c r="I4" s="1"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="21"/>
-      <c r="T4" s="1"/>
+      <c r="Q4" s="21"/>
+      <c r="S4" s="1"/>
+      <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
+      <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
-      <c r="AK4" s="3"/>
+      <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
-      <c r="AN4" s="2"/>
-    </row>
-    <row r="5" spans="1:43">
-      <c r="J5" s="1"/>
+    </row>
+    <row r="5" spans="1:42">
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="L5" s="9"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="21"/>
-      <c r="T5" s="1"/>
+      <c r="Q5" s="21"/>
+      <c r="S5" s="1"/>
+      <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
+      <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
-      <c r="AK5" s="3"/>
+      <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
-      <c r="AN5" s="2"/>
-    </row>
-    <row r="6" spans="1:43">
-      <c r="J6" s="1"/>
+    </row>
+    <row r="6" spans="1:42">
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="21"/>
-      <c r="T6" s="1"/>
+      <c r="Q6" s="21"/>
+      <c r="S6" s="1"/>
+      <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
+      <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
+      <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
-      <c r="AN6" s="2"/>
-    </row>
-    <row r="7" spans="1:43">
-      <c r="J7" s="1"/>
+    </row>
+    <row r="7" spans="1:42">
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
+      <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="21"/>
-      <c r="T7" s="1"/>
+      <c r="Q7" s="21"/>
+      <c r="S7" s="1"/>
+      <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
+      <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
+      <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
-    </row>
-    <row r="8" spans="1:43">
-      <c r="J8" s="1"/>
+    </row>
+    <row r="8" spans="1:42">
+      <c r="I8" s="1"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
+      <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="21"/>
-      <c r="T8" s="1"/>
+      <c r="Q8" s="21"/>
+      <c r="S8" s="1"/>
+      <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
+      <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
+      <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
       <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-    </row>
-    <row r="9" spans="1:43">
-      <c r="J9" s="1"/>
+    </row>
+    <row r="9" spans="1:42">
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
+      <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="21"/>
-      <c r="T9" s="1"/>
+      <c r="Q9" s="21"/>
+      <c r="S9" s="1"/>
+      <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
+      <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
-      <c r="AK9" s="3"/>
+      <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
-      <c r="AN9" s="2"/>
-    </row>
-    <row r="10" spans="1:43">
-      <c r="J10" s="1"/>
+    </row>
+    <row r="10" spans="1:42">
+      <c r="I10" s="1"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
+      <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="21"/>
-      <c r="T10" s="1"/>
+      <c r="Q10" s="21"/>
+      <c r="S10" s="1"/>
+      <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
+      <c r="AE10" s="3"/>
       <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
+      <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
       <c r="AM10" s="2"/>
-      <c r="AN10" s="2"/>
-    </row>
-    <row r="11" spans="1:43">
+    </row>
+    <row r="11" spans="1:42">
+      <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="R11" s="21"/>
-    </row>
-    <row r="12" spans="1:43">
+      <c r="Q11" s="21"/>
+    </row>
+    <row r="12" spans="1:42">
+      <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="R12" s="21"/>
-    </row>
-    <row r="13" spans="1:43">
+      <c r="Q12" s="21"/>
+    </row>
+    <row r="13" spans="1:42">
+      <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="R13" s="21"/>
-    </row>
-    <row r="14" spans="1:43">
+      <c r="Q13" s="21"/>
+    </row>
+    <row r="14" spans="1:42">
+      <c r="L14" s="10"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="R14" s="21"/>
-    </row>
-    <row r="15" spans="1:43">
+      <c r="Q14" s="21"/>
+    </row>
+    <row r="15" spans="1:42">
+      <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="R15" s="21"/>
-    </row>
-    <row r="16" spans="1:43">
+      <c r="Q15" s="21"/>
+    </row>
+    <row r="16" spans="1:42">
+      <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="R16" s="21"/>
-    </row>
-    <row r="17" spans="13:18">
+      <c r="Q16" s="21"/>
+    </row>
+    <row r="17" spans="12:17">
+      <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="R17" s="21"/>
-    </row>
-    <row r="18" spans="13:18">
+      <c r="Q17" s="21"/>
+    </row>
+    <row r="18" spans="12:17">
+      <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="R18" s="21"/>
-    </row>
-    <row r="19" spans="13:18">
+      <c r="Q18" s="21"/>
+    </row>
+    <row r="19" spans="12:17">
+      <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="R19" s="21"/>
-    </row>
-    <row r="20" spans="13:18">
+      <c r="Q19" s="21"/>
+    </row>
+    <row r="20" spans="12:17">
+      <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="R20" s="21"/>
-    </row>
-    <row r="21" spans="13:18">
+      <c r="Q20" s="21"/>
+    </row>
+    <row r="21" spans="12:17">
+      <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="R21" s="21"/>
-    </row>
-    <row r="22" spans="13:18">
+      <c r="Q21" s="21"/>
+    </row>
+    <row r="22" spans="12:17">
+      <c r="L22" s="10"/>
       <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="R22" s="21"/>
-    </row>
-    <row r="23" spans="13:18">
+      <c r="Q22" s="21"/>
+    </row>
+    <row r="23" spans="12:17">
+      <c r="L23" s="10"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="R23" s="21"/>
-    </row>
-    <row r="24" spans="13:18">
+      <c r="Q23" s="21"/>
+    </row>
+    <row r="24" spans="12:17">
+      <c r="L24" s="10"/>
       <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="R24" s="21"/>
-    </row>
-    <row r="25" spans="13:18">
+      <c r="Q24" s="21"/>
+    </row>
+    <row r="25" spans="12:17">
+      <c r="L25" s="10"/>
       <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="R25" s="21"/>
-    </row>
-    <row r="26" spans="13:18">
+      <c r="Q25" s="21"/>
+    </row>
+    <row r="26" spans="12:17">
+      <c r="L26" s="10"/>
       <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="R26" s="21"/>
-    </row>
-    <row r="27" spans="13:18">
+      <c r="Q26" s="21"/>
+    </row>
+    <row r="27" spans="12:17">
+      <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="R27" s="21"/>
-    </row>
-    <row r="28" spans="13:18">
+      <c r="Q27" s="21"/>
+    </row>
+    <row r="28" spans="12:17">
+      <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="R28" s="21"/>
-    </row>
-    <row r="29" spans="13:18">
+      <c r="Q28" s="21"/>
+    </row>
+    <row r="29" spans="12:17">
+      <c r="L29" s="10"/>
       <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="R29" s="21"/>
-    </row>
-    <row r="30" spans="13:18">
+      <c r="Q29" s="21"/>
+    </row>
+    <row r="30" spans="12:17">
+      <c r="L30" s="10"/>
       <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="R30" s="21"/>
-    </row>
-    <row r="31" spans="13:18">
+      <c r="Q30" s="21"/>
+    </row>
+    <row r="31" spans="12:17">
+      <c r="L31" s="10"/>
       <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="R31" s="21"/>
-    </row>
-    <row r="32" spans="13:18">
+      <c r="Q31" s="21"/>
+    </row>
+    <row r="32" spans="12:17">
+      <c r="L32" s="10"/>
       <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="R32" s="21"/>
-    </row>
-    <row r="33" spans="13:18">
+      <c r="Q32" s="21"/>
+    </row>
+    <row r="33" spans="12:17">
+      <c r="L33" s="10"/>
       <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="R33" s="21"/>
-    </row>
-    <row r="34" spans="13:18">
+      <c r="Q33" s="21"/>
+    </row>
+    <row r="34" spans="12:17">
+      <c r="L34" s="10"/>
       <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="R34" s="21"/>
-    </row>
-    <row r="35" spans="13:18">
+      <c r="Q34" s="21"/>
+    </row>
+    <row r="35" spans="12:17">
+      <c r="L35" s="10"/>
       <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="R35" s="21"/>
-    </row>
-    <row r="36" spans="13:18">
+      <c r="Q35" s="21"/>
+    </row>
+    <row r="36" spans="12:17">
+      <c r="L36" s="10"/>
       <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="R36" s="21"/>
-    </row>
-    <row r="37" spans="13:18">
+      <c r="Q36" s="21"/>
+    </row>
+    <row r="37" spans="12:17">
+      <c r="L37" s="10"/>
       <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="R37" s="21"/>
-    </row>
-    <row r="38" spans="13:18">
+      <c r="Q37" s="21"/>
+    </row>
+    <row r="38" spans="12:17">
+      <c r="L38" s="10"/>
       <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="R38" s="21"/>
-    </row>
-    <row r="39" spans="13:18">
+      <c r="Q38" s="21"/>
+    </row>
+    <row r="39" spans="12:17">
+      <c r="L39" s="10"/>
       <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="R39" s="21"/>
-    </row>
-    <row r="40" spans="13:18">
+      <c r="Q39" s="21"/>
+    </row>
+    <row r="40" spans="12:17">
+      <c r="L40" s="10"/>
       <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="R40" s="21"/>
-    </row>
-    <row r="41" spans="13:18">
+      <c r="Q40" s="21"/>
+    </row>
+    <row r="41" spans="12:17">
+      <c r="L41" s="10"/>
       <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="R41" s="21"/>
-    </row>
-    <row r="42" spans="13:18">
+      <c r="Q41" s="21"/>
+    </row>
+    <row r="42" spans="12:17">
+      <c r="L42" s="10"/>
       <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="R42" s="21"/>
-    </row>
-    <row r="43" spans="13:18">
+      <c r="Q42" s="21"/>
+    </row>
+    <row r="43" spans="12:17">
+      <c r="L43" s="10"/>
       <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="R43" s="21"/>
-    </row>
-    <row r="44" spans="13:18">
+      <c r="Q43" s="21"/>
+    </row>
+    <row r="44" spans="12:17">
+      <c r="L44" s="10"/>
       <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="R44" s="21"/>
-    </row>
-    <row r="45" spans="13:18">
+      <c r="Q44" s="21"/>
+    </row>
+    <row r="45" spans="12:17">
+      <c r="L45" s="10"/>
       <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="R45" s="21"/>
-    </row>
-    <row r="46" spans="13:18">
+      <c r="Q45" s="21"/>
+    </row>
+    <row r="46" spans="12:17">
+      <c r="L46" s="10"/>
       <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="R46" s="21"/>
-    </row>
-    <row r="47" spans="13:18">
+      <c r="Q46" s="21"/>
+    </row>
+    <row r="47" spans="12:17">
+      <c r="L47" s="10"/>
       <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-      <c r="R47" s="21"/>
-    </row>
-    <row r="48" spans="13:18">
+      <c r="Q47" s="21"/>
+    </row>
+    <row r="48" spans="12:17">
+      <c r="L48" s="10"/>
       <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-      <c r="R48" s="21"/>
-    </row>
-    <row r="49" spans="13:18">
+      <c r="Q48" s="21"/>
+    </row>
+    <row r="49" spans="12:17">
+      <c r="L49" s="10"/>
       <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-      <c r="R49" s="21"/>
+      <c r="Q49" s="21"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM1048576 AC1:AC1048576 AL1:AL1048576 AN1:AN1048576 AQ1 AO2:AQ1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL1048576 AB1:AB1048576 AK1:AK1048576 AM1:AM1048576 AP1 AN2:AP1048576">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
       <formula1>"Male,Female,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
       <formula1>"Married,UnMarried,Single"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>